<commit_message>
Pixel Sensitivity. Amalgamation of pilot 3 data.
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Release/Pilots and trials/Pilot 3/Subject 14 - roiy pilot.xlsx
+++ b/FilmFinder/FilmFinder/bin/Release/Pilots and trials/Pilot 3/Subject 14 - roiy pilot.xlsx
@@ -734,11 +734,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112677248"/>
-        <c:axId val="112678784"/>
+        <c:axId val="127832448"/>
+        <c:axId val="127833984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112677248"/>
+        <c:axId val="127832448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112678784"/>
+        <c:crossAx val="127833984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -755,7 +755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112678784"/>
+        <c:axId val="127833984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112677248"/>
+        <c:crossAx val="127832448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1130,11 +1130,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112710400"/>
-        <c:axId val="112711936"/>
+        <c:axId val="128074496"/>
+        <c:axId val="128076032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112710400"/>
+        <c:axId val="128074496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112711936"/>
+        <c:crossAx val="128076032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1151,7 +1151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112711936"/>
+        <c:axId val="128076032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1162,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112710400"/>
+        <c:crossAx val="128074496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1526,11 +1526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="117457664"/>
-        <c:axId val="117459200"/>
+        <c:axId val="128135936"/>
+        <c:axId val="128137472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117457664"/>
+        <c:axId val="128135936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +1539,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117459200"/>
+        <c:crossAx val="128137472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1547,7 +1547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117459200"/>
+        <c:axId val="128137472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117457664"/>
+        <c:crossAx val="128135936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1964,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>